<commit_message>
improved formatting of test data for the test oneWayFlightFilters
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/oneWayFlightFilters.xlsx
+++ b/src/test/resources/datasheets/oneWayFlightFilters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bajwauto\Projects\MultiAppPOM\multiApp\src\test\resources\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C268071D-155E-4CB2-A210-58774805A56A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76487A45-3351-4A09-AD40-6BC3FB9ECCFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>sourceCity</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Onward Price</t>
+  </si>
+  <si>
+    <t>1-1-21</t>
   </si>
 </sst>
 </file>
@@ -116,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -125,9 +128,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -413,7 +413,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,8 +498,8 @@
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4">
-        <v>44197</v>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>

</xml_diff>